<commit_message>
fix: old predictions cleanup, dropping odds reset, git push flow
</commit_message>
<xml_diff>
--- a/filtered/gunun_surprizleri_20.02.2026.xlsx
+++ b/filtered/gunun_surprizleri_20.02.2026.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>home_team</t>
   </si>
@@ -31,70 +31,16 @@
     <t>ms_5_5_ust</t>
   </si>
   <si>
-    <t>Shabab Al Ahli</t>
-  </si>
-  <si>
-    <t>Atalanta</t>
-  </si>
-  <si>
-    <t>Famalicao</t>
-  </si>
-  <si>
-    <t>Celtic</t>
-  </si>
-  <si>
-    <t>Az Alkmaar</t>
-  </si>
-  <si>
-    <t>Psv Eindhoven</t>
-  </si>
-  <si>
-    <t>Karabağ</t>
-  </si>
-  <si>
     <t>Nordsjaelland</t>
   </si>
   <si>
     <t>Helmond</t>
   </si>
   <si>
-    <t>Al Hilal (Riyad</t>
-  </si>
-  <si>
-    <t>Cremonese</t>
-  </si>
-  <si>
-    <t>Avs</t>
-  </si>
-  <si>
-    <t>Dundee Utd</t>
-  </si>
-  <si>
-    <t>Volendam</t>
-  </si>
-  <si>
-    <t>Excelsior</t>
-  </si>
-  <si>
-    <t>Newcastle</t>
-  </si>
-  <si>
     <t>Vejle</t>
   </si>
   <si>
     <t>Den Haag</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>20:30</t>
-  </si>
-  <si>
-    <t>21:45</t>
-  </si>
-  <si>
-    <t>20:45</t>
   </si>
   <si>
     <t>21:00</t>
@@ -461,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,16 +435,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>2.07</v>
+        <v>6.98</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -506,125 +452,15 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4">
-        <v>2.68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5">
-        <v>5.17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6">
-        <v>4.42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7">
-        <v>3.39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9">
-        <v>6.98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10">
         <v>5.72</v>
       </c>
     </row>

</xml_diff>